<commit_message>
Added a submission folder. Report just needs screenshots
</commit_message>
<xml_diff>
--- a/Paperwork/sprint-backlog.xlsx
+++ b/Paperwork/sprint-backlog.xlsx
@@ -5,26 +5,27 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kurty\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ronsc_000\Documents\GitHub\PotatoApp\Paperwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="643" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="643" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProductBacklog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint Backlog" sheetId="2" r:id="rId2"/>
-    <sheet name="Acceptance Tests" sheetId="4" r:id="rId3"/>
-    <sheet name="user_stories" sheetId="5" r:id="rId4"/>
-    <sheet name="UserStories" sheetId="6" r:id="rId5"/>
-    <sheet name="Configuration Details" sheetId="7" r:id="rId6"/>
+    <sheet name="Burndown Chart" sheetId="8" r:id="rId3"/>
+    <sheet name="Acceptance Tests" sheetId="4" r:id="rId4"/>
+    <sheet name="user_stories" sheetId="5" r:id="rId5"/>
+    <sheet name="UserStories" sheetId="6" r:id="rId6"/>
+    <sheet name="Configuration Details" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="133">
   <si>
     <t>ID</t>
   </si>
@@ -185,16 +186,10 @@
     <t>KM</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Create Database tables</t>
   </si>
   <si>
     <t>populate DB</t>
-  </si>
-  <si>
-    <t>Not Started</t>
   </si>
   <si>
     <t>Create Stored Procedures</t>
@@ -439,7 +434,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -493,6 +488,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="186"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -799,7 +800,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -862,6 +862,9 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -899,6 +902,999 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Date</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Burndown</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="35000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Sprint Backlog'!$F$40:$R$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="368455984"/>
+        <c:axId val="368461864"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="368455984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Date</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="[$-407]d/\ mmm/\ yyyy;@" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="368461864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="368461864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Hours</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="368455984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1242,7 +2238,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D2" s="30" t="s">
         <v>10</v>
@@ -1261,7 +2257,7 @@
         <v>100</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1285,7 +2281,7 @@
         <v>9</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>12</v>
@@ -1304,7 +2300,7 @@
         <v>70</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J3" s="14"/>
       <c r="K3" s="1"/>
@@ -1328,7 +2324,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>13</v>
@@ -1345,7 +2341,7 @@
         <v>210</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="1"/>
@@ -1367,10 +2363,10 @@
         <v>9</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11">
@@ -1383,7 +2379,7 @@
         <v>80</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="1"/>
@@ -1405,10 +2401,10 @@
         <v>9</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11">
@@ -1421,7 +2417,7 @@
         <v>80</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J6" s="14"/>
       <c r="K6" s="1"/>
@@ -1442,7 +2438,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -1457,7 +2453,7 @@
         <v>80</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="38.25" x14ac:dyDescent="0.2">
@@ -1755,10 +2751,10 @@
         <v>23</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E15" s="18"/>
       <c r="F15" s="2">
@@ -1772,7 +2768,7 @@
         <v>600</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="J15" s="14"/>
       <c r="K15" s="1"/>
@@ -3953,8 +4949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="B20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4023,40 +5019,40 @@
       <c r="O3" s="33"/>
     </row>
     <row r="4" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="77" t="s">
+      <c r="D4" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="77" t="s">
+      <c r="E4" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="74" t="s">
+      <c r="F4" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="75"/>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
-      <c r="M4" s="75"/>
-      <c r="N4" s="75"/>
-      <c r="O4" s="76"/>
+      <c r="G4" s="74"/>
+      <c r="H4" s="74"/>
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="74"/>
+      <c r="O4" s="75"/>
     </row>
     <row r="5" spans="1:18" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="78"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
+      <c r="A5" s="77"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
       <c r="F5" s="34" t="s">
         <v>37</v>
       </c>
@@ -4098,11 +5094,11 @@
       </c>
     </row>
     <row r="6" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="79"/>
-      <c r="B6" s="79"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
+      <c r="A6" s="78"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
+      <c r="E6" s="78"/>
       <c r="F6" s="35">
         <f>WORKDAY('Configuration Details'!$B$1,INT(RIGHT(F5,2)))</f>
         <v>41899</v>
@@ -4248,7 +5244,7 @@
         <v>52</v>
       </c>
       <c r="D9" s="44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E9" s="45"/>
       <c r="F9" s="42">
@@ -4278,14 +5274,22 @@
       <c r="N9" s="42">
         <v>8</v>
       </c>
-      <c r="O9" s="42"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="42"/>
-      <c r="R9" s="42"/>
+      <c r="O9" s="42">
+        <v>4</v>
+      </c>
+      <c r="P9" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="42">
+        <v>0</v>
+      </c>
+      <c r="R9" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="42">
         <v>5</v>
@@ -4294,7 +5298,7 @@
         <v>52</v>
       </c>
       <c r="D10" s="44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E10" s="45"/>
       <c r="F10" s="42">
@@ -4324,14 +5328,22 @@
       <c r="N10" s="42">
         <v>4</v>
       </c>
-      <c r="O10" s="42"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="42"/>
-      <c r="R10" s="42"/>
+      <c r="O10" s="42">
+        <v>3</v>
+      </c>
+      <c r="P10" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="42">
+        <v>0</v>
+      </c>
+      <c r="R10" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="42">
         <v>15</v>
@@ -4340,7 +5352,7 @@
         <v>52</v>
       </c>
       <c r="D11" s="44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E11" s="45"/>
       <c r="F11" s="42">
@@ -4370,14 +5382,22 @@
       <c r="N11" s="42">
         <v>3</v>
       </c>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="42"/>
-      <c r="R11" s="42"/>
+      <c r="O11" s="42">
+        <v>0</v>
+      </c>
+      <c r="P11" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="42">
+        <v>0</v>
+      </c>
+      <c r="R11" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B12" s="42">
         <v>9</v>
@@ -4386,7 +5406,7 @@
         <v>52</v>
       </c>
       <c r="D12" s="44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E12" s="45"/>
       <c r="F12" s="42">
@@ -4401,7 +5421,9 @@
       <c r="I12" s="42">
         <v>5</v>
       </c>
-      <c r="J12" s="42"/>
+      <c r="J12" s="42">
+        <v>3</v>
+      </c>
       <c r="K12" s="42">
         <v>5</v>
       </c>
@@ -4414,23 +5436,31 @@
       <c r="N12" s="42">
         <v>4</v>
       </c>
-      <c r="O12" s="42"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="42"/>
-      <c r="R12" s="42"/>
+      <c r="O12" s="42">
+        <v>2</v>
+      </c>
+      <c r="P12" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="42">
+        <v>0</v>
+      </c>
+      <c r="R12" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B13" s="42">
         <v>30</v>
       </c>
       <c r="C13" s="43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D13" s="44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E13" s="45"/>
       <c r="F13" s="42">
@@ -4460,23 +5490,31 @@
       <c r="N13" s="42">
         <v>9</v>
       </c>
-      <c r="O13" s="42"/>
-      <c r="P13" s="42"/>
-      <c r="Q13" s="42"/>
-      <c r="R13" s="42"/>
+      <c r="O13" s="42">
+        <v>5</v>
+      </c>
+      <c r="P13" s="42">
+        <v>3</v>
+      </c>
+      <c r="Q13" s="42">
+        <v>0</v>
+      </c>
+      <c r="R13" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B14" s="42">
         <v>1</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D14" s="44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E14" s="45"/>
       <c r="F14" s="42">
@@ -4506,21 +5544,29 @@
       <c r="N14" s="42">
         <v>9</v>
       </c>
-      <c r="O14" s="42"/>
-      <c r="P14" s="42"/>
-      <c r="Q14" s="42"/>
-      <c r="R14" s="42"/>
+      <c r="O14" s="42">
+        <v>4</v>
+      </c>
+      <c r="P14" s="42">
+        <v>4</v>
+      </c>
+      <c r="Q14" s="42">
+        <v>0</v>
+      </c>
+      <c r="R14" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:18" s="26" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B15" s="46"/>
       <c r="C15" s="47" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D15" s="48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E15" s="40"/>
       <c r="F15" s="46"/>
@@ -4539,16 +5585,16 @@
     </row>
     <row r="16" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B16" s="42">
         <v>1</v>
       </c>
       <c r="C16" s="43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D16" s="44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E16" s="45"/>
       <c r="F16" s="42">
@@ -4578,21 +5624,29 @@
       <c r="N16" s="42">
         <v>1</v>
       </c>
-      <c r="O16" s="42"/>
-      <c r="P16" s="42"/>
-      <c r="Q16" s="42"/>
-      <c r="R16" s="42"/>
+      <c r="O16" s="42">
+        <v>0</v>
+      </c>
+      <c r="P16" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="42">
+        <v>0</v>
+      </c>
+      <c r="R16" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:18" s="26" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B17" s="46"/>
       <c r="C17" s="47" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D17" s="48" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E17" s="40"/>
       <c r="F17" s="46"/>
@@ -4611,16 +5665,16 @@
     </row>
     <row r="18" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B18" s="42">
         <v>1</v>
       </c>
       <c r="C18" s="43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D18" s="44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E18" s="45"/>
       <c r="F18" s="42">
@@ -4650,18 +5704,26 @@
       <c r="N18" s="42">
         <v>1</v>
       </c>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="42"/>
+      <c r="O18" s="42">
+        <v>0</v>
+      </c>
+      <c r="P18" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="42">
+        <v>0</v>
+      </c>
+      <c r="R18" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:18" s="26" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A19" s="26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B19" s="46"/>
       <c r="C19" s="47" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D19" s="48"/>
       <c r="E19" s="40"/>
@@ -4681,16 +5743,16 @@
     </row>
     <row r="20" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B20" s="42">
         <v>5</v>
       </c>
       <c r="C20" s="43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D20" s="44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E20" s="45"/>
       <c r="F20" s="42">
@@ -4720,23 +5782,31 @@
       <c r="N20" s="42">
         <v>2</v>
       </c>
-      <c r="O20" s="42"/>
-      <c r="P20" s="42"/>
-      <c r="Q20" s="42"/>
-      <c r="R20" s="42"/>
+      <c r="O20" s="42">
+        <v>0</v>
+      </c>
+      <c r="P20" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="42">
+        <v>0</v>
+      </c>
+      <c r="R20" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B21" s="42">
         <v>10</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D21" s="44" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="E21" s="45"/>
       <c r="F21" s="42">
@@ -4745,25 +5815,47 @@
       <c r="G21" s="42">
         <v>10</v>
       </c>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="L21" s="42"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="42"/>
-      <c r="P21" s="42"/>
-      <c r="Q21" s="42"/>
-      <c r="R21" s="42"/>
+      <c r="H21" s="42">
+        <v>10</v>
+      </c>
+      <c r="I21" s="42">
+        <v>10</v>
+      </c>
+      <c r="J21" s="42">
+        <v>10</v>
+      </c>
+      <c r="K21" s="42">
+        <v>4</v>
+      </c>
+      <c r="L21" s="42">
+        <v>4</v>
+      </c>
+      <c r="M21" s="42">
+        <v>2</v>
+      </c>
+      <c r="N21" s="42">
+        <v>0</v>
+      </c>
+      <c r="O21" s="42">
+        <v>0</v>
+      </c>
+      <c r="P21" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="42">
+        <v>0</v>
+      </c>
+      <c r="R21" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:18" s="26" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" s="46"/>
       <c r="C22" s="47" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D22" s="48"/>
       <c r="E22" s="40"/>
@@ -4783,16 +5875,16 @@
     </row>
     <row r="23" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B23" s="42">
         <v>1</v>
       </c>
       <c r="C23" s="43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D23" s="44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E23" s="45"/>
       <c r="F23" s="42">
@@ -4804,29 +5896,49 @@
       <c r="H23" s="42">
         <v>0</v>
       </c>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-      <c r="L23" s="42"/>
-      <c r="M23" s="42"/>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42"/>
-      <c r="P23" s="42"/>
-      <c r="Q23" s="42"/>
-      <c r="R23" s="42"/>
+      <c r="I23" s="42">
+        <v>0</v>
+      </c>
+      <c r="J23" s="42">
+        <v>0</v>
+      </c>
+      <c r="K23" s="42">
+        <v>0</v>
+      </c>
+      <c r="L23" s="42">
+        <v>0</v>
+      </c>
+      <c r="M23" s="42">
+        <v>0</v>
+      </c>
+      <c r="N23" s="42">
+        <v>0</v>
+      </c>
+      <c r="O23" s="42">
+        <v>0</v>
+      </c>
+      <c r="P23" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="42">
+        <v>0</v>
+      </c>
+      <c r="R23" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B24" s="42">
         <v>2</v>
       </c>
       <c r="C24" s="43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D24" s="44" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E24" s="45"/>
       <c r="F24" s="42">
@@ -4835,30 +5947,52 @@
       <c r="G24" s="42">
         <v>2</v>
       </c>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
-      <c r="P24" s="42"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="42"/>
+      <c r="H24" s="42">
+        <v>5</v>
+      </c>
+      <c r="I24" s="42">
+        <v>2</v>
+      </c>
+      <c r="J24" s="42">
+        <v>1</v>
+      </c>
+      <c r="K24" s="42">
+        <v>0</v>
+      </c>
+      <c r="L24" s="42">
+        <v>0</v>
+      </c>
+      <c r="M24" s="42">
+        <v>0</v>
+      </c>
+      <c r="N24" s="42">
+        <v>0</v>
+      </c>
+      <c r="O24" s="42">
+        <v>0</v>
+      </c>
+      <c r="P24" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="42">
+        <v>0</v>
+      </c>
+      <c r="R24" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B25" s="42">
         <v>2</v>
       </c>
       <c r="C25" s="43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D25" s="44" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="E25" s="45"/>
       <c r="F25" s="42">
@@ -4867,21 +6001,43 @@
       <c r="G25" s="42">
         <v>2</v>
       </c>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
-      <c r="N25" s="42"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="42"/>
-      <c r="Q25" s="42"/>
-      <c r="R25" s="42"/>
+      <c r="H25" s="42">
+        <v>4</v>
+      </c>
+      <c r="I25" s="42">
+        <v>3</v>
+      </c>
+      <c r="J25" s="42">
+        <v>2</v>
+      </c>
+      <c r="K25" s="42">
+        <v>1</v>
+      </c>
+      <c r="L25" s="42">
+        <v>0</v>
+      </c>
+      <c r="M25" s="42">
+        <v>0</v>
+      </c>
+      <c r="N25" s="42">
+        <v>0</v>
+      </c>
+      <c r="O25" s="42">
+        <v>0</v>
+      </c>
+      <c r="P25" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="42">
+        <v>0</v>
+      </c>
+      <c r="R25" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:18" s="26" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A26" s="26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B26" s="46"/>
       <c r="C26" s="47"/>
@@ -4903,39 +6059,61 @@
     </row>
     <row r="27" spans="1:18" s="24" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B27" s="49">
         <v>2</v>
       </c>
       <c r="C27" s="50" t="s">
-        <v>133</v>
-      </c>
-      <c r="D27" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="52"/>
+        <v>131</v>
+      </c>
+      <c r="D27" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="51"/>
       <c r="F27" s="49">
         <v>2</v>
       </c>
       <c r="G27" s="49">
         <v>2</v>
       </c>
-      <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="49"/>
-      <c r="K27" s="49"/>
-      <c r="L27" s="49"/>
-      <c r="M27" s="49"/>
-      <c r="N27" s="49"/>
-      <c r="O27" s="49"/>
-      <c r="P27" s="49"/>
-      <c r="Q27" s="49"/>
-      <c r="R27" s="49"/>
+      <c r="H27" s="49">
+        <v>2</v>
+      </c>
+      <c r="I27" s="49">
+        <v>2</v>
+      </c>
+      <c r="J27" s="49">
+        <v>2</v>
+      </c>
+      <c r="K27" s="49">
+        <v>2</v>
+      </c>
+      <c r="L27" s="49">
+        <v>2</v>
+      </c>
+      <c r="M27" s="49">
+        <v>2</v>
+      </c>
+      <c r="N27" s="49">
+        <v>2</v>
+      </c>
+      <c r="O27" s="49">
+        <v>1</v>
+      </c>
+      <c r="P27" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="42">
+        <v>0</v>
+      </c>
+      <c r="R27" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:18" s="26" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B28" s="46"/>
       <c r="C28" s="47"/>
@@ -4957,103 +6135,169 @@
     </row>
     <row r="29" spans="1:18" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B29" s="49">
         <v>1</v>
       </c>
       <c r="C29" s="50" t="s">
-        <v>133</v>
-      </c>
-      <c r="D29" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="E29" s="52"/>
+        <v>131</v>
+      </c>
+      <c r="D29" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="51"/>
       <c r="F29" s="49">
         <v>1</v>
       </c>
       <c r="G29" s="49">
         <v>1</v>
       </c>
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="49"/>
-      <c r="K29" s="49"/>
-      <c r="L29" s="49"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="49"/>
-      <c r="O29" s="49"/>
-      <c r="P29" s="49"/>
-      <c r="Q29" s="49"/>
-      <c r="R29" s="49"/>
+      <c r="H29" s="49">
+        <v>1</v>
+      </c>
+      <c r="I29" s="49">
+        <v>1</v>
+      </c>
+      <c r="J29" s="49">
+        <v>1</v>
+      </c>
+      <c r="K29" s="49">
+        <v>1</v>
+      </c>
+      <c r="L29" s="49">
+        <v>1</v>
+      </c>
+      <c r="M29" s="49">
+        <v>1</v>
+      </c>
+      <c r="N29" s="49">
+        <v>0</v>
+      </c>
+      <c r="O29" s="49">
+        <v>0</v>
+      </c>
+      <c r="P29" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="42">
+        <v>0</v>
+      </c>
+      <c r="R29" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:18" s="24" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B30" s="49">
         <v>2</v>
       </c>
       <c r="C30" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="D30" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" s="52"/>
+        <v>132</v>
+      </c>
+      <c r="D30" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="E30" s="51"/>
       <c r="F30" s="49">
         <v>2</v>
       </c>
       <c r="G30" s="49">
         <v>2</v>
       </c>
-      <c r="H30" s="49"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="49"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49"/>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
-      <c r="Q30" s="49"/>
-      <c r="R30" s="49"/>
+      <c r="H30" s="49">
+        <v>2</v>
+      </c>
+      <c r="I30" s="49">
+        <v>2</v>
+      </c>
+      <c r="J30" s="49">
+        <v>2</v>
+      </c>
+      <c r="K30" s="49">
+        <v>1</v>
+      </c>
+      <c r="L30" s="49">
+        <v>1</v>
+      </c>
+      <c r="M30" s="49">
+        <v>0</v>
+      </c>
+      <c r="N30" s="49">
+        <v>0</v>
+      </c>
+      <c r="O30" s="49">
+        <v>0</v>
+      </c>
+      <c r="P30" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="42">
+        <v>0</v>
+      </c>
+      <c r="R30" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:18" s="24" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B31" s="49">
         <v>2</v>
       </c>
       <c r="C31" s="50" t="s">
-        <v>134</v>
-      </c>
-      <c r="D31" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="52"/>
+        <v>132</v>
+      </c>
+      <c r="D31" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="51"/>
       <c r="F31" s="49">
         <v>2</v>
       </c>
       <c r="G31" s="49">
         <v>2</v>
       </c>
-      <c r="H31" s="49"/>
-      <c r="I31" s="49"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="49"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="49"/>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="49"/>
-      <c r="R31" s="49"/>
+      <c r="H31" s="49">
+        <v>2</v>
+      </c>
+      <c r="I31" s="49">
+        <v>2</v>
+      </c>
+      <c r="J31" s="49">
+        <v>2</v>
+      </c>
+      <c r="K31" s="42">
+        <v>0</v>
+      </c>
+      <c r="L31" s="42">
+        <v>0</v>
+      </c>
+      <c r="M31" s="42">
+        <v>0</v>
+      </c>
+      <c r="N31" s="42">
+        <v>0</v>
+      </c>
+      <c r="O31" s="42">
+        <v>0</v>
+      </c>
+      <c r="P31" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="42">
+        <v>0</v>
+      </c>
+      <c r="R31" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:18" s="26" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B32" s="46"/>
       <c r="C32" s="47"/>
@@ -5075,48 +6319,70 @@
     </row>
     <row r="33" spans="1:18" s="24" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B33" s="49">
         <v>10</v>
       </c>
       <c r="C33" s="50" t="s">
-        <v>117</v>
-      </c>
-      <c r="D33" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" s="52"/>
+        <v>115</v>
+      </c>
+      <c r="D33" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="E33" s="51"/>
       <c r="F33" s="49">
         <v>10</v>
       </c>
       <c r="G33" s="49">
         <v>8</v>
       </c>
-      <c r="H33" s="49"/>
-      <c r="I33" s="49"/>
-      <c r="J33" s="49"/>
-      <c r="K33" s="49"/>
-      <c r="L33" s="49"/>
-      <c r="M33" s="49"/>
-      <c r="N33" s="49"/>
-      <c r="O33" s="49"/>
-      <c r="P33" s="49"/>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="49"/>
+      <c r="H33" s="49">
+        <v>8</v>
+      </c>
+      <c r="I33" s="49">
+        <v>8</v>
+      </c>
+      <c r="J33" s="49">
+        <v>8</v>
+      </c>
+      <c r="K33" s="49">
+        <v>4</v>
+      </c>
+      <c r="L33" s="49">
+        <v>4</v>
+      </c>
+      <c r="M33" s="49">
+        <v>4</v>
+      </c>
+      <c r="N33" s="49">
+        <v>2</v>
+      </c>
+      <c r="O33" s="49">
+        <v>1</v>
+      </c>
+      <c r="P33" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="42">
+        <v>0</v>
+      </c>
+      <c r="R33" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B34" s="42">
         <v>10</v>
       </c>
       <c r="C34" s="43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D34" s="44" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="E34" s="45"/>
       <c r="F34" s="42">
@@ -5125,21 +6391,43 @@
       <c r="G34" s="42">
         <v>10</v>
       </c>
-      <c r="H34" s="42"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="42"/>
-      <c r="L34" s="42"/>
-      <c r="M34" s="42"/>
-      <c r="N34" s="42"/>
-      <c r="O34" s="42"/>
-      <c r="P34" s="42"/>
-      <c r="Q34" s="42"/>
-      <c r="R34" s="42"/>
+      <c r="H34" s="42">
+        <v>10</v>
+      </c>
+      <c r="I34" s="42">
+        <v>7</v>
+      </c>
+      <c r="J34" s="42">
+        <v>5</v>
+      </c>
+      <c r="K34" s="42">
+        <v>5</v>
+      </c>
+      <c r="L34" s="42">
+        <v>3</v>
+      </c>
+      <c r="M34" s="42">
+        <v>1</v>
+      </c>
+      <c r="N34" s="42">
+        <v>3</v>
+      </c>
+      <c r="O34" s="42">
+        <v>0</v>
+      </c>
+      <c r="P34" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="42">
+        <v>0</v>
+      </c>
+      <c r="R34" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:18" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A35" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B35" s="40"/>
       <c r="C35" s="40"/>
@@ -5161,16 +6449,16 @@
     </row>
     <row r="36" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B36" s="42">
         <v>5</v>
       </c>
       <c r="C36" s="43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D36" s="44" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="E36" s="45"/>
       <c r="F36" s="42">
@@ -5179,21 +6467,43 @@
       <c r="G36" s="42">
         <v>5</v>
       </c>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="42"/>
-      <c r="K36" s="42"/>
-      <c r="L36" s="42"/>
-      <c r="M36" s="42"/>
-      <c r="N36" s="42"/>
-      <c r="O36" s="42"/>
-      <c r="P36" s="42"/>
-      <c r="Q36" s="42"/>
-      <c r="R36" s="42"/>
+      <c r="H36" s="42">
+        <v>4</v>
+      </c>
+      <c r="I36" s="42">
+        <v>4</v>
+      </c>
+      <c r="J36" s="42">
+        <v>3</v>
+      </c>
+      <c r="K36" s="42">
+        <v>2</v>
+      </c>
+      <c r="L36" s="42">
+        <v>1</v>
+      </c>
+      <c r="M36" s="42">
+        <v>0</v>
+      </c>
+      <c r="N36" s="42">
+        <v>0</v>
+      </c>
+      <c r="O36" s="42">
+        <v>0</v>
+      </c>
+      <c r="P36" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="42">
+        <v>0</v>
+      </c>
+      <c r="R36" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:18" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B37" s="40"/>
       <c r="C37" s="40"/>
@@ -5214,17 +6524,17 @@
       <c r="R37" s="41"/>
     </row>
     <row r="38" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="53" t="s">
-        <v>85</v>
+      <c r="A38" s="52" t="s">
+        <v>83</v>
       </c>
       <c r="B38" s="42">
         <v>10</v>
       </c>
       <c r="C38" s="43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D38" s="44" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="E38" s="45"/>
       <c r="F38" s="42">
@@ -5233,20 +6543,42 @@
       <c r="G38" s="42">
         <v>9</v>
       </c>
-      <c r="H38" s="42"/>
-      <c r="I38" s="42"/>
-      <c r="J38" s="42"/>
-      <c r="K38" s="42"/>
-      <c r="L38" s="42"/>
-      <c r="M38" s="42"/>
-      <c r="N38" s="42"/>
-      <c r="O38" s="42"/>
-      <c r="P38" s="42"/>
-      <c r="Q38" s="42"/>
-      <c r="R38" s="42"/>
+      <c r="H38" s="42">
+        <v>9</v>
+      </c>
+      <c r="I38" s="42">
+        <v>7</v>
+      </c>
+      <c r="J38" s="42">
+        <v>6</v>
+      </c>
+      <c r="K38" s="42">
+        <v>4</v>
+      </c>
+      <c r="L38" s="42">
+        <v>4</v>
+      </c>
+      <c r="M38" s="42">
+        <v>5</v>
+      </c>
+      <c r="N38" s="42">
+        <v>4</v>
+      </c>
+      <c r="O38" s="42">
+        <v>2</v>
+      </c>
+      <c r="P38" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="42">
+        <v>0</v>
+      </c>
+      <c r="R38" s="42">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="53"/>
+      <c r="A39" s="52"/>
       <c r="B39" s="42"/>
       <c r="C39" s="43"/>
       <c r="D39" s="44"/>
@@ -5266,62 +6598,62 @@
       <c r="R39" s="42"/>
     </row>
     <row r="40" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="54"/>
-      <c r="B40" s="54"/>
-      <c r="C40" s="54"/>
-      <c r="D40" s="55"/>
-      <c r="E40" s="56" t="s">
-        <v>86</v>
-      </c>
-      <c r="F40" s="56">
+      <c r="A40" s="53"/>
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="54"/>
+      <c r="E40" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="F40" s="55">
         <f>SUM(F9:F39)</f>
         <v>129</v>
       </c>
-      <c r="G40" s="56">
+      <c r="G40" s="55">
         <f t="shared" ref="G40:L40" si="3">SUM(G9:G39)</f>
         <v>115</v>
       </c>
-      <c r="H40" s="56">
+      <c r="H40" s="55">
         <f t="shared" si="3"/>
-        <v>60</v>
-      </c>
-      <c r="I40" s="56">
+        <v>117</v>
+      </c>
+      <c r="I40" s="55">
         <f t="shared" si="3"/>
-        <v>54</v>
-      </c>
-      <c r="J40" s="56">
+        <v>102</v>
+      </c>
+      <c r="J40" s="55">
         <f t="shared" si="3"/>
-        <v>30</v>
-      </c>
-      <c r="K40" s="56">
+        <v>75</v>
+      </c>
+      <c r="K40" s="55">
         <f t="shared" si="3"/>
-        <v>48</v>
-      </c>
-      <c r="L40" s="56">
+        <v>72</v>
+      </c>
+      <c r="L40" s="55">
         <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="M40" s="56">
+        <v>70</v>
+      </c>
+      <c r="M40" s="55">
         <f t="shared" ref="M40" si="4">SUM(M9:M39)</f>
-        <v>46</v>
-      </c>
-      <c r="N40" s="56">
+        <v>61</v>
+      </c>
+      <c r="N40" s="55">
         <f t="shared" ref="N40" si="5">SUM(N9:N39)</f>
-        <v>41</v>
-      </c>
-      <c r="O40" s="56">
+        <v>52</v>
+      </c>
+      <c r="O40" s="55">
         <f t="shared" ref="O40" si="6">SUM(O9:O39)</f>
-        <v>0</v>
-      </c>
-      <c r="P40" s="56">
+        <v>22</v>
+      </c>
+      <c r="P40" s="55">
         <f t="shared" ref="P40" si="7">SUM(P9:P39)</f>
-        <v>0</v>
-      </c>
-      <c r="Q40" s="56">
+        <v>7</v>
+      </c>
+      <c r="Q40" s="55">
         <f t="shared" ref="Q40" si="8">SUM(Q9:Q39)</f>
         <v>0</v>
       </c>
-      <c r="R40" s="56">
+      <c r="R40" s="55">
         <f t="shared" ref="R40" si="9">SUM(R9:R39)</f>
         <v>0</v>
       </c>
@@ -5330,9 +6662,9 @@
       <c r="A41" s="33"/>
       <c r="B41" s="33"/>
       <c r="C41" s="33"/>
-      <c r="D41" s="57"/>
+      <c r="D41" s="56"/>
       <c r="E41" s="44" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F41" s="44"/>
       <c r="G41" s="44">
@@ -5341,43 +6673,43 @@
       </c>
       <c r="H41" s="44">
         <f t="shared" ref="H41:P41" si="10">G40-H40</f>
-        <v>55</v>
+        <v>-2</v>
       </c>
       <c r="I41" s="44">
         <f t="shared" si="10"/>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="J41" s="44">
         <f t="shared" si="10"/>
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="K41" s="44">
         <f t="shared" si="10"/>
-        <v>-18</v>
+        <v>3</v>
       </c>
       <c r="L41" s="44">
         <f t="shared" si="10"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="M41" s="44">
         <f t="shared" si="10"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="N41" s="44">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="O41" s="44">
         <f t="shared" si="10"/>
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="P41" s="44">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="Q41" s="44">
         <f t="shared" ref="Q41" si="11">P40-Q40</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R41" s="44">
         <f t="shared" ref="R41" si="12">Q40-R40</f>
@@ -5385,33 +6717,33 @@
       </c>
     </row>
     <row r="42" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="58" t="s">
-        <v>88</v>
+      <c r="A42" s="57" t="s">
+        <v>86</v>
       </c>
       <c r="B42" s="5">
         <f>SUM(B9:B40)</f>
         <v>129</v>
       </c>
-      <c r="C42" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="D42" s="60"/>
-      <c r="E42" s="54"/>
-      <c r="F42" s="54"/>
-      <c r="G42" s="54"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="54"/>
-      <c r="K42" s="54"/>
-      <c r="L42" s="54"/>
-      <c r="M42" s="54"/>
-      <c r="N42" s="54"/>
-      <c r="O42" s="54"/>
+      <c r="C42" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="D42" s="59"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="53"/>
+      <c r="L42" s="53"/>
+      <c r="M42" s="53"/>
+      <c r="N42" s="53"/>
+      <c r="O42" s="53"/>
     </row>
     <row r="43" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="61"/>
-      <c r="B43" s="62"/>
-      <c r="C43" s="54"/>
+      <c r="A43" s="60"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="53"/>
       <c r="D43" s="32"/>
       <c r="E43" s="32"/>
       <c r="F43" s="32"/>
@@ -5426,11 +6758,11 @@
       <c r="O43" s="32"/>
     </row>
     <row r="44" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="63" t="s">
-        <v>90</v>
+      <c r="A44" s="62" t="s">
+        <v>88</v>
       </c>
       <c r="B44" s="44"/>
-      <c r="C44" s="60"/>
+      <c r="C44" s="59"/>
       <c r="D44" s="32"/>
       <c r="E44" s="32"/>
       <c r="F44" s="32"/>
@@ -5446,13 +6778,13 @@
     </row>
     <row r="45" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B45" s="44">
         <f>COUNTIF($D$9:$D$40,"Not Started")</f>
-        <v>3</v>
-      </c>
-      <c r="C45" s="60"/>
+        <v>0</v>
+      </c>
+      <c r="C45" s="59"/>
       <c r="D45" s="32"/>
       <c r="E45" s="32"/>
       <c r="F45" s="32"/>
@@ -5468,13 +6800,13 @@
     </row>
     <row r="46" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B46" s="44">
         <f>COUNTIF($D$9:$D$40,"In Progress")</f>
-        <v>7</v>
-      </c>
-      <c r="C46" s="60"/>
+        <v>0</v>
+      </c>
+      <c r="C46" s="59"/>
       <c r="D46" s="32"/>
       <c r="E46" s="32"/>
       <c r="F46" s="32"/>
@@ -5490,13 +6822,13 @@
     </row>
     <row r="47" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B47" s="44">
         <f>COUNTIF($D$9:$D$40,"Complete")</f>
-        <v>13</v>
-      </c>
-      <c r="C47" s="60"/>
+        <v>23</v>
+      </c>
+      <c r="C47" s="59"/>
       <c r="D47" s="32"/>
       <c r="E47" s="32"/>
       <c r="F47" s="32"/>
@@ -5511,8 +6843,8 @@
       <c r="O47" s="32"/>
     </row>
     <row r="48" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="54"/>
-      <c r="B48" s="54"/>
+      <c r="A48" s="53"/>
+      <c r="B48" s="53"/>
       <c r="C48" s="32"/>
       <c r="D48" s="32"/>
       <c r="E48" s="32"/>
@@ -5537,7 +6869,7 @@
     <mergeCell ref="E4:E6"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D38:D39 D36 D9:D34">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D36 D9:D34 D38:D39">
       <formula1>"Not Started,In Progress,Complete,"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5638,6 +6970,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D7:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="7" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="79"/>
+    </row>
+    <row r="13" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D13" s="79"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -5653,133 +7008,133 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="65" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="65" t="s">
-        <v>96</v>
-      </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="67"/>
+      <c r="E1" s="66"/>
     </row>
     <row r="2" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
-      <c r="E2" s="67"/>
+      <c r="E2" s="66"/>
     </row>
     <row r="3" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="27"/>
-      <c r="E3" s="67"/>
+      <c r="E3" s="66"/>
     </row>
     <row r="4" spans="1:5" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27"/>
-      <c r="E4" s="67"/>
+      <c r="E4" s="66"/>
     </row>
     <row r="5" spans="1:5" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27"/>
-      <c r="E5" s="67"/>
+      <c r="E5" s="66"/>
     </row>
     <row r="6" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="27"/>
-      <c r="E6" s="67"/>
+      <c r="E6" s="66"/>
     </row>
     <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
-      <c r="E7" s="67"/>
+      <c r="E7" s="66"/>
     </row>
     <row r="8" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="27"/>
-      <c r="E8" s="67"/>
+      <c r="E8" s="66"/>
     </row>
     <row r="9" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C9" s="27"/>
       <c r="D9" s="27"/>
-      <c r="E9" s="67"/>
+      <c r="E9" s="66"/>
     </row>
     <row r="10" spans="1:5" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C10" s="27"/>
       <c r="D10" s="27"/>
-      <c r="E10" s="67"/>
+      <c r="E10" s="66"/>
     </row>
     <row r="11" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="67"/>
+      <c r="E11" s="66"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="68" t="s">
-        <v>109</v>
+      <c r="A12" s="67" t="s">
+        <v>107</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -5951,7 +7306,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -5968,8 +7323,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
-        <v>110</v>
+      <c r="A1" s="68" t="s">
+        <v>108</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -5985,7 +7340,7 @@
     </row>
     <row r="3" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="22"/>
@@ -5993,7 +7348,7 @@
     </row>
     <row r="4" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" s="22"/>
@@ -6001,7 +7356,7 @@
     </row>
     <row r="5" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -6009,7 +7364,7 @@
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -6017,7 +7372,7 @@
     </row>
     <row r="7" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -6025,7 +7380,7 @@
     </row>
     <row r="8" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -6033,7 +7388,7 @@
     </row>
     <row r="9" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -6041,7 +7396,7 @@
     </row>
     <row r="10" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -6049,7 +7404,7 @@
     </row>
     <row r="11" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -6065,7 +7420,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A97"/>
   <sheetViews>
@@ -6663,7 +8018,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
@@ -6677,10 +8032,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="70" t="s">
-        <v>111</v>
-      </c>
-      <c r="B1" s="71">
+      <c r="A1" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="70">
         <v>41899</v>
       </c>
       <c r="C1" s="32"/>
@@ -6697,48 +8052,48 @@
       <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
-        <v>112</v>
-      </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="60"/>
+      <c r="A3" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="71"/>
+      <c r="C3" s="59"/>
       <c r="D3" s="32"/>
       <c r="E3" s="32"/>
       <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C4" s="8"/>
-      <c r="D4" s="73"/>
+      <c r="D4" s="72"/>
       <c r="E4" s="32"/>
       <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C5" s="8"/>
-      <c r="D5" s="73"/>
+      <c r="D5" s="72"/>
       <c r="E5" s="32"/>
       <c r="F5" s="32"/>
     </row>
     <row r="6" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C6" s="8"/>
-      <c r="D6" s="73"/>
+      <c r="D6" s="72"/>
       <c r="E6" s="32"/>
       <c r="F6" s="32"/>
     </row>
@@ -6747,58 +8102,58 @@
         <v>52</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C7" s="8"/>
-      <c r="D7" s="73"/>
+      <c r="D7" s="72"/>
       <c r="E7" s="32"/>
       <c r="F7" s="32"/>
     </row>
     <row r="8" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C8" s="8"/>
-      <c r="D8" s="73"/>
+      <c r="D8" s="72"/>
       <c r="E8" s="32"/>
       <c r="F8" s="32"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="8"/>
-      <c r="D9" s="73"/>
+      <c r="D9" s="72"/>
       <c r="E9" s="32"/>
       <c r="F9" s="32"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="73"/>
+      <c r="D10" s="72"/>
       <c r="E10" s="32"/>
       <c r="F10" s="32"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="73" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" s="73"/>
-      <c r="C11" s="73"/>
+      <c r="A11" s="72" t="s">
+        <v>132</v>
+      </c>
+      <c r="B11" s="72"/>
+      <c r="C11" s="72"/>
       <c r="D11" s="32"/>
       <c r="E11" s="32"/>
       <c r="F11" s="32"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B12" s="32"/>
       <c r="C12" s="32"/>

</xml_diff>